<commit_message>
nova funcionalidade no planejamento
</commit_message>
<xml_diff>
--- a/documentos/outros-documentos/Sprint-4/planejamento-sprint4.xlsx
+++ b/documentos/outros-documentos/Sprint-4/planejamento-sprint4.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>SPRINT 3:</t>
   </si>
@@ -62,6 +62,9 @@
   <si>
     <t>Estória de Usuário: CH:2 ID:11 – Excluir Trabalhos (MATHEUS)</t>
   </si>
+  <si>
+    <t>Estória de Usuário: CH:2 ID:11 – Segurança de Navegação (MATHEUS)</t>
+  </si>
 </sst>
 </file>
 
@@ -70,7 +73,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -156,6 +159,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF3333"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -271,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -354,6 +364,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -755,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:F17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -19320,14 +19333,14 @@
       <c r="AMJ20"/>
     </row>
     <row r="21" spans="1:1024">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
       <c r="G21" s="7"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
@@ -21490,12 +21503,14 @@
       <c r="Z26" s="23"/>
     </row>
     <row r="27" spans="1:1024" s="24" customFormat="1" ht="13.5">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+      <c r="A27" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
       <c r="G27" s="17"/>
       <c r="H27" s="8"/>
       <c r="I27" s="22"/>
@@ -21601,11 +21616,12 @@
       <c r="Y30" s="22"/>
       <c r="Z30" s="23"/>
     </row>
-    <row r="34" spans="5:5" ht="409.6">
+    <row r="34" spans="5:5">
       <c r="E34" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="A27:F27"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A25:F25"/>
     <mergeCell ref="A13:F13"/>

</xml_diff>

<commit_message>
criterios de aceitação eliana
</commit_message>
<xml_diff>
--- a/documentos/outros-documentos/Sprint-4/planejamento-sprint4.xlsx
+++ b/documentos/outros-documentos/Sprint-4/planejamento-sprint4.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="62">
   <si>
     <t>SPRINT 3:</t>
   </si>
@@ -140,12 +140,78 @@
   <si>
     <t>2 hora</t>
   </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>Incrementar diagrama de classe</t>
+  </si>
+  <si>
+    <t>Alterar classe loginBean</t>
+  </si>
+  <si>
+    <t>Criar página esqueciMinhaSenha</t>
+  </si>
+  <si>
+    <t>Integração + Testes</t>
+  </si>
+  <si>
+    <t>criar classe CSS</t>
+  </si>
+  <si>
+    <t>criar metodo avaliarProfissional</t>
+  </si>
+  <si>
+    <t>Integração + testes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cauê </t>
+  </si>
+  <si>
+    <t>30 minutos</t>
+  </si>
+  <si>
+    <t>1 Hora</t>
+  </si>
+  <si>
+    <t>3 Horas</t>
+  </si>
+  <si>
+    <t>Criar pagina com localização por area</t>
+  </si>
+  <si>
+    <t>implementar api google por distancia</t>
+  </si>
+  <si>
+    <t>integração, testes</t>
+  </si>
+  <si>
+    <t>Estória de Usuário: CH:9 ID:42 – Mobile (Igor Bruno)</t>
+  </si>
+  <si>
+    <t>Passar todas as paginas para prime faces mobile</t>
+  </si>
+  <si>
+    <t>Igor e Bruno</t>
+  </si>
+  <si>
+    <t>20 horas</t>
+  </si>
+  <si>
+    <t>IGOR</t>
+  </si>
+  <si>
+    <t>4 horas</t>
+  </si>
+  <si>
+    <t>Integração e testes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -247,6 +313,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -379,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -425,12 +498,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -487,6 +554,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -884,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK32"/>
+  <dimension ref="A1:AMK64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:F28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3989,12 +4085,12 @@
       <c r="AMJ3"/>
     </row>
     <row r="4" spans="1:1024" ht="15" thickBot="1">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
       <c r="G4" s="7"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -5015,14 +5111,14 @@
       <c r="AMJ4"/>
     </row>
     <row r="5" spans="1:1024" ht="15" thickBot="1">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -6043,28 +6139,28 @@
       <c r="AMJ5"/>
     </row>
     <row r="6" spans="1:1024" ht="15" thickBot="1">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="20" t="s">
         <v>16</v>
       </c>
       <c r="I6" s="8"/>
@@ -6093,17 +6189,17 @@
       <c r="AF6"/>
       <c r="AG6"/>
       <c r="AH6"/>
-      <c r="AI6" s="24"/>
-      <c r="AJ6" s="24"/>
-      <c r="AK6" s="24"/>
-      <c r="AL6" s="24"/>
-      <c r="AM6" s="24"/>
-      <c r="AN6" s="24"/>
-      <c r="AO6" s="24"/>
-      <c r="AP6" s="24"/>
-      <c r="AQ6" s="24"/>
-      <c r="AR6" s="24"/>
-      <c r="AS6" s="24"/>
+      <c r="AI6" s="22"/>
+      <c r="AJ6" s="22"/>
+      <c r="AK6" s="22"/>
+      <c r="AL6" s="22"/>
+      <c r="AM6" s="22"/>
+      <c r="AN6" s="22"/>
+      <c r="AO6" s="22"/>
+      <c r="AP6" s="22"/>
+      <c r="AQ6" s="22"/>
+      <c r="AR6" s="22"/>
+      <c r="AS6" s="22"/>
       <c r="AT6"/>
       <c r="AU6"/>
       <c r="AV6"/>
@@ -7085,22 +7181,22 @@
       <c r="AMJ6"/>
     </row>
     <row r="7" spans="1:1024" ht="15" thickBot="1">
-      <c r="A7" s="27">
+      <c r="A7" s="25">
         <v>1</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="24">
         <v>42524</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="24">
         <v>42524</v>
       </c>
       <c r="G7" s="7"/>
@@ -7131,17 +7227,17 @@
       <c r="AF7"/>
       <c r="AG7"/>
       <c r="AH7"/>
-      <c r="AI7" s="24"/>
-      <c r="AJ7" s="24"/>
-      <c r="AK7" s="24"/>
-      <c r="AL7" s="24"/>
-      <c r="AM7" s="24"/>
-      <c r="AN7" s="24"/>
-      <c r="AO7" s="24"/>
-      <c r="AP7" s="24"/>
-      <c r="AQ7" s="24"/>
-      <c r="AR7" s="24"/>
-      <c r="AS7" s="24"/>
+      <c r="AI7" s="22"/>
+      <c r="AJ7" s="22"/>
+      <c r="AK7" s="22"/>
+      <c r="AL7" s="22"/>
+      <c r="AM7" s="22"/>
+      <c r="AN7" s="22"/>
+      <c r="AO7" s="22"/>
+      <c r="AP7" s="22"/>
+      <c r="AQ7" s="22"/>
+      <c r="AR7" s="22"/>
+      <c r="AS7" s="22"/>
       <c r="AT7"/>
       <c r="AU7"/>
       <c r="AV7"/>
@@ -8123,22 +8219,22 @@
       <c r="AMJ7"/>
     </row>
     <row r="8" spans="1:1024" ht="40.5" customHeight="1" thickBot="1">
-      <c r="A8" s="28">
+      <c r="A8" s="26">
         <v>2</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="24">
         <v>42525</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="24">
         <v>42525</v>
       </c>
       <c r="G8" s="7" t="s">
@@ -8171,17 +8267,17 @@
       <c r="AF8"/>
       <c r="AG8"/>
       <c r="AH8"/>
-      <c r="AI8" s="24"/>
-      <c r="AJ8" s="24"/>
-      <c r="AK8" s="24"/>
-      <c r="AL8" s="24"/>
-      <c r="AM8" s="24"/>
-      <c r="AN8" s="24"/>
-      <c r="AO8" s="24"/>
-      <c r="AP8" s="24"/>
-      <c r="AQ8" s="24"/>
-      <c r="AR8" s="24"/>
-      <c r="AS8" s="24"/>
+      <c r="AI8" s="22"/>
+      <c r="AJ8" s="22"/>
+      <c r="AK8" s="22"/>
+      <c r="AL8" s="22"/>
+      <c r="AM8" s="22"/>
+      <c r="AN8" s="22"/>
+      <c r="AO8" s="22"/>
+      <c r="AP8" s="22"/>
+      <c r="AQ8" s="22"/>
+      <c r="AR8" s="22"/>
+      <c r="AS8" s="22"/>
       <c r="AT8"/>
       <c r="AU8"/>
       <c r="AV8"/>
@@ -9163,22 +9259,22 @@
       <c r="AMJ8"/>
     </row>
     <row r="9" spans="1:1024" ht="15" thickBot="1">
-      <c r="A9" s="27">
+      <c r="A9" s="25">
         <v>3</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="24">
         <v>42527</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="24">
         <v>42527</v>
       </c>
       <c r="G9" s="7"/>
@@ -9209,17 +9305,17 @@
       <c r="AF9"/>
       <c r="AG9"/>
       <c r="AH9"/>
-      <c r="AI9" s="24"/>
-      <c r="AJ9" s="24"/>
-      <c r="AK9" s="24"/>
-      <c r="AL9" s="24"/>
-      <c r="AM9" s="24"/>
-      <c r="AN9" s="24"/>
-      <c r="AO9" s="24"/>
-      <c r="AP9" s="24"/>
-      <c r="AQ9" s="24"/>
-      <c r="AR9" s="24"/>
-      <c r="AS9" s="24"/>
+      <c r="AI9" s="22"/>
+      <c r="AJ9" s="22"/>
+      <c r="AK9" s="22"/>
+      <c r="AL9" s="22"/>
+      <c r="AM9" s="22"/>
+      <c r="AN9" s="22"/>
+      <c r="AO9" s="22"/>
+      <c r="AP9" s="22"/>
+      <c r="AQ9" s="22"/>
+      <c r="AR9" s="22"/>
+      <c r="AS9" s="22"/>
       <c r="AT9"/>
       <c r="AU9"/>
       <c r="AV9"/>
@@ -10201,22 +10297,22 @@
       <c r="AMJ9"/>
     </row>
     <row r="10" spans="1:1024" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A10" s="28">
+      <c r="A10" s="26">
         <v>4</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="24">
         <v>42527</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="24">
         <v>42527</v>
       </c>
       <c r="G10" s="7" t="s">
@@ -10249,17 +10345,17 @@
       <c r="AF10"/>
       <c r="AG10"/>
       <c r="AH10"/>
-      <c r="AI10" s="24"/>
-      <c r="AJ10" s="24"/>
-      <c r="AK10" s="24"/>
-      <c r="AL10" s="24"/>
-      <c r="AM10" s="24"/>
-      <c r="AN10" s="24"/>
-      <c r="AO10" s="24"/>
-      <c r="AP10" s="24"/>
-      <c r="AQ10" s="24"/>
-      <c r="AR10" s="24"/>
-      <c r="AS10" s="24"/>
+      <c r="AI10" s="22"/>
+      <c r="AJ10" s="22"/>
+      <c r="AK10" s="22"/>
+      <c r="AL10" s="22"/>
+      <c r="AM10" s="22"/>
+      <c r="AN10" s="22"/>
+      <c r="AO10" s="22"/>
+      <c r="AP10" s="22"/>
+      <c r="AQ10" s="22"/>
+      <c r="AR10" s="22"/>
+      <c r="AS10" s="22"/>
       <c r="AT10"/>
       <c r="AU10"/>
       <c r="AV10"/>
@@ -11241,22 +11337,22 @@
       <c r="AMJ10"/>
     </row>
     <row r="11" spans="1:1024" ht="15" thickBot="1">
-      <c r="A11" s="27">
+      <c r="A11" s="25">
         <v>5</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="24">
         <v>42528</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="24">
         <v>42528</v>
       </c>
       <c r="G11" s="7" t="s">
@@ -11289,17 +11385,17 @@
       <c r="AF11"/>
       <c r="AG11"/>
       <c r="AH11"/>
-      <c r="AI11" s="24"/>
-      <c r="AJ11" s="24"/>
-      <c r="AK11" s="24"/>
-      <c r="AL11" s="24"/>
-      <c r="AM11" s="24"/>
-      <c r="AN11" s="24"/>
-      <c r="AO11" s="24"/>
-      <c r="AP11" s="24"/>
-      <c r="AQ11" s="24"/>
-      <c r="AR11" s="24"/>
-      <c r="AS11" s="24"/>
+      <c r="AI11" s="22"/>
+      <c r="AJ11" s="22"/>
+      <c r="AK11" s="22"/>
+      <c r="AL11" s="22"/>
+      <c r="AM11" s="22"/>
+      <c r="AN11" s="22"/>
+      <c r="AO11" s="22"/>
+      <c r="AP11" s="22"/>
+      <c r="AQ11" s="22"/>
+      <c r="AR11" s="22"/>
+      <c r="AS11" s="22"/>
       <c r="AT11"/>
       <c r="AU11"/>
       <c r="AV11"/>
@@ -12281,25 +12377,25 @@
       <c r="AMJ11"/>
     </row>
     <row r="12" spans="1:1024" s="17" customFormat="1" ht="15" thickBot="1">
-      <c r="A12" s="31">
+      <c r="A12" s="29">
         <v>6</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="33">
         <v>42528</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="33">
         <v>42528</v>
       </c>
-      <c r="G12" s="30"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="18"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -12321,25 +12417,25 @@
       <c r="Z12" s="15"/>
     </row>
     <row r="13" spans="1:1024" s="17" customFormat="1" ht="15" thickBot="1">
-      <c r="A13" s="31">
+      <c r="A13" s="29">
         <v>7</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="31">
         <v>42528</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="31">
         <v>42528</v>
       </c>
-      <c r="G13" s="30"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="18"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
@@ -12361,8 +12457,8 @@
       <c r="Z13" s="15"/>
     </row>
     <row r="14" spans="1:1024" s="17" customFormat="1" ht="15" thickBot="1">
-      <c r="A14" s="29"/>
-      <c r="G14" s="30"/>
+      <c r="A14" s="27"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="18"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -12384,14 +12480,14 @@
       <c r="Z14" s="15"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -13412,28 +13508,28 @@
       <c r="AMJ15"/>
     </row>
     <row r="16" spans="1:1024" s="11" customFormat="1" thickBot="1">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="20" t="s">
         <v>16</v>
       </c>
       <c r="I16" s="10"/>
@@ -13456,22 +13552,22 @@
       <c r="Z16" s="9"/>
     </row>
     <row r="17" spans="1:1024" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A17" s="27">
+      <c r="A17" s="25">
         <v>8</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="24">
         <v>42530</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="24">
         <v>42530</v>
       </c>
       <c r="G17" s="7"/>
@@ -14494,22 +14590,22 @@
       <c r="AMJ17"/>
     </row>
     <row r="18" spans="1:1024" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A18" s="28">
+      <c r="A18" s="26">
         <v>9</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="24">
         <v>42530</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="24">
         <v>42530</v>
       </c>
       <c r="G18" s="7" t="s">
@@ -15534,22 +15630,22 @@
       <c r="AMJ18"/>
     </row>
     <row r="19" spans="1:1024" ht="15" customHeight="1" thickBot="1">
-      <c r="A19" s="27">
+      <c r="A19" s="25">
         <v>10</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="24">
         <v>42530</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="24">
         <v>42531</v>
       </c>
       <c r="G19" s="7"/>
@@ -16572,22 +16668,22 @@
       <c r="AMJ19"/>
     </row>
     <row r="20" spans="1:1024" ht="26.25" thickBot="1">
-      <c r="A20" s="28">
+      <c r="A20" s="26">
         <v>11</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="24">
         <v>42532</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="24">
         <v>42532</v>
       </c>
       <c r="G20" s="7" t="s">
@@ -17612,7 +17708,7 @@
       <c r="AMJ20"/>
     </row>
     <row r="21" spans="1:1024" ht="15" thickBot="1">
-      <c r="A21" s="27">
+      <c r="A21" s="25">
         <v>12</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -17624,10 +17720,10 @@
       <c r="D21" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="36">
+      <c r="E21" s="34">
         <v>42532</v>
       </c>
-      <c r="F21" s="36">
+      <c r="F21" s="34">
         <v>42532</v>
       </c>
       <c r="G21" s="7"/>
@@ -18650,22 +18746,22 @@
       <c r="AMJ21"/>
     </row>
     <row r="22" spans="1:1024" ht="15" thickBot="1">
-      <c r="A22" s="27">
+      <c r="A22" s="25">
         <v>13</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="24">
         <v>42532</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="24">
         <v>42532</v>
       </c>
       <c r="G22" s="7"/>
@@ -20709,14 +20805,14 @@
       <c r="AMJ23"/>
     </row>
     <row r="24" spans="1:1024" ht="15" thickBot="1">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
       <c r="G24" s="13"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -21737,28 +21833,28 @@
       <c r="AMJ24"/>
     </row>
     <row r="25" spans="1:1024" ht="15" thickBot="1">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="23" t="s">
+      <c r="G25" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="20" t="s">
         <v>16</v>
       </c>
       <c r="I25" s="8"/>
@@ -22779,22 +22875,22 @@
       <c r="AMJ25"/>
     </row>
     <row r="26" spans="1:1024" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A26" s="27">
+      <c r="A26" s="25">
         <v>14</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="24">
         <v>42533</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="24">
         <v>42533</v>
       </c>
       <c r="G26" s="7"/>
@@ -22819,72 +22915,566 @@
       <c r="Z26" s="15"/>
     </row>
     <row r="27" spans="1:1024" ht="15" thickBot="1">
-      <c r="A27" s="27"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="38"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="36"/>
     </row>
     <row r="28" spans="1:1024" ht="15" thickBot="1">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:1024" ht="15" thickBot="1">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
+      <c r="A29" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="30" spans="1:1024" ht="15" thickBot="1">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="23">
+        <v>15</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="24">
+        <v>42524</v>
+      </c>
+      <c r="F30" s="45">
+        <v>42527</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1024" ht="15" thickBot="1">
+      <c r="A31" s="23">
+        <v>16</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="24">
+        <v>42524</v>
+      </c>
+      <c r="F31" s="45">
+        <v>42527</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1024" ht="15" thickBot="1">
+      <c r="A32" s="43">
+        <v>17</v>
+      </c>
+      <c r="B32" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="24">
+        <v>42524</v>
+      </c>
+      <c r="F32" s="45">
+        <v>42527</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="43">
+        <v>18</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="45">
+        <v>42527</v>
+      </c>
+      <c r="F33" s="45">
+        <v>42527</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" thickBot="1"/>
+    <row r="35" spans="1:8" ht="15" thickBot="1">
+      <c r="A35" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
     </row>
-    <row r="31" spans="1:1024" ht="15" thickBot="1">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
+    <row r="36" spans="1:8" ht="15" thickBot="1">
+      <c r="A36" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="32" spans="1:1024" ht="15" thickBot="1">
-      <c r="A32" s="19" t="s">
+    <row r="37" spans="1:8" ht="15" thickBot="1">
+      <c r="A37" s="32">
+        <v>19</v>
+      </c>
+      <c r="B37" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="44">
+        <v>42527</v>
+      </c>
+      <c r="F37" s="44">
+        <v>42533</v>
+      </c>
+      <c r="G37" s="41"/>
+      <c r="H37" s="42"/>
+    </row>
+    <row r="38" spans="1:8" ht="15" thickBot="1">
+      <c r="A38" s="32">
+        <v>20</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="44">
+        <v>42527</v>
+      </c>
+      <c r="F38" s="44">
+        <v>42533</v>
+      </c>
+      <c r="G38" s="41"/>
+      <c r="H38" s="42"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1">
+      <c r="A39" s="32">
+        <v>21</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="44">
+        <v>42529</v>
+      </c>
+      <c r="F39" s="44">
+        <v>42533</v>
+      </c>
+      <c r="G39" s="41"/>
+      <c r="H39" s="42"/>
+    </row>
+    <row r="40" spans="1:8" ht="15" thickBot="1">
+      <c r="A40" s="40"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="42"/>
+    </row>
+    <row r="41" spans="1:8" ht="15" thickBot="1">
+      <c r="A41" s="40"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="42"/>
+    </row>
+    <row r="42" spans="1:8" ht="15" thickBot="1">
+      <c r="A42" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+    </row>
+    <row r="43" spans="1:8" ht="15" thickBot="1">
+      <c r="A43" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="1">
+        <v>22</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="47">
+        <v>42435</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="1">
+        <v>23</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="1">
+        <v>24</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15" thickBot="1"/>
+    <row r="48" spans="1:8" ht="15" thickBot="1">
+      <c r="A48" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+    </row>
+    <row r="49" spans="1:1025" ht="15" thickBot="1">
+      <c r="A49" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1025">
+      <c r="A50" s="1">
+        <v>25</v>
+      </c>
+      <c r="B50" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E50" s="47">
+        <v>42527</v>
+      </c>
+      <c r="F50" s="47">
+        <v>42541</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1025">
+      <c r="A51" s="1">
+        <v>26</v>
+      </c>
+      <c r="B51" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="47">
+        <v>42527</v>
+      </c>
+      <c r="F51" s="47">
+        <v>42541</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1025">
+      <c r="D53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="AMD53"/>
+      <c r="AME53"/>
+      <c r="AMF53"/>
+      <c r="AMG53"/>
+      <c r="AMH53"/>
+      <c r="AMI53"/>
+      <c r="AMJ53"/>
+      <c r="AMK53"/>
+    </row>
+    <row r="54" spans="1:1025">
+      <c r="D54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="AMD54"/>
+      <c r="AME54"/>
+      <c r="AMF54"/>
+      <c r="AMG54"/>
+      <c r="AMH54"/>
+      <c r="AMI54"/>
+      <c r="AMJ54"/>
+      <c r="AMK54"/>
+    </row>
+    <row r="55" spans="1:1025">
+      <c r="D55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="AMD55"/>
+      <c r="AME55"/>
+      <c r="AMF55"/>
+      <c r="AMG55"/>
+      <c r="AMH55"/>
+      <c r="AMI55"/>
+      <c r="AMJ55"/>
+      <c r="AMK55"/>
+    </row>
+    <row r="56" spans="1:1025">
+      <c r="D56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="AMD56"/>
+      <c r="AME56"/>
+      <c r="AMF56"/>
+      <c r="AMG56"/>
+      <c r="AMH56"/>
+      <c r="AMI56"/>
+      <c r="AMJ56"/>
+      <c r="AMK56"/>
+    </row>
+    <row r="57" spans="1:1025">
+      <c r="D57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="AMD57"/>
+      <c r="AME57"/>
+      <c r="AMF57"/>
+      <c r="AMG57"/>
+      <c r="AMH57"/>
+      <c r="AMI57"/>
+      <c r="AMJ57"/>
+      <c r="AMK57"/>
+    </row>
+    <row r="58" spans="1:1025">
+      <c r="D58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="AMD58"/>
+      <c r="AME58"/>
+      <c r="AMF58"/>
+      <c r="AMG58"/>
+      <c r="AMH58"/>
+      <c r="AMI58"/>
+      <c r="AMJ58"/>
+      <c r="AMK58"/>
+    </row>
+    <row r="59" spans="1:1025">
+      <c r="D59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="AMD59"/>
+      <c r="AME59"/>
+      <c r="AMF59"/>
+      <c r="AMG59"/>
+      <c r="AMH59"/>
+      <c r="AMI59"/>
+      <c r="AMJ59"/>
+      <c r="AMK59"/>
+    </row>
+    <row r="60" spans="1:1025">
+      <c r="D60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="AMD60"/>
+      <c r="AME60"/>
+      <c r="AMF60"/>
+      <c r="AMG60"/>
+      <c r="AMH60"/>
+      <c r="AMI60"/>
+      <c r="AMJ60"/>
+      <c r="AMK60"/>
+    </row>
+    <row r="61" spans="1:1025">
+      <c r="D61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="AMD61"/>
+      <c r="AME61"/>
+      <c r="AMF61"/>
+      <c r="AMG61"/>
+      <c r="AMH61"/>
+      <c r="AMI61"/>
+      <c r="AMJ61"/>
+      <c r="AMK61"/>
+    </row>
+    <row r="62" spans="1:1025">
+      <c r="D62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="AMD62"/>
+      <c r="AME62"/>
+      <c r="AMF62"/>
+      <c r="AMG62"/>
+      <c r="AMH62"/>
+      <c r="AMI62"/>
+      <c r="AMJ62"/>
+      <c r="AMK62"/>
+    </row>
+    <row r="63" spans="1:1025">
+      <c r="D63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="AMD63"/>
+      <c r="AME63"/>
+      <c r="AMF63"/>
+      <c r="AMG63"/>
+      <c r="AMH63"/>
+      <c r="AMI63"/>
+      <c r="AMJ63"/>
+      <c r="AMK63"/>
+    </row>
+    <row r="64" spans="1:1025">
+      <c r="D64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="AMD64"/>
+      <c r="AME64"/>
+      <c r="AMF64"/>
+      <c r="AMG64"/>
+      <c r="AMH64"/>
+      <c r="AMI64"/>
+      <c r="AMJ64"/>
+      <c r="AMK64"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A29:F29"/>
+  <mergeCells count="8">
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A28:F28"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.13888888888888901" bottom="0.13888888888888901" header="0" footer="0"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>